<commit_message>
Add Net Zero by 2050 mitigation scenario
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SYS_ZeroCO2_2050.xlsx
+++ b/SuppXLS/Scen_SYS_ZeroCO2_2050.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DABF9267-E133-412D-A1B2-0EE3B5C9556A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F25FD08-7D51-4F02-A34E-10DBB506647D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="config" sheetId="20" r:id="rId2"/>
     <sheet name="single" sheetId="21" r:id="rId3"/>
     <sheet name="multi" sheetId="22" r:id="rId4"/>
+    <sheet name="negative_CO2" sheetId="23" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="__123Graph_AEUMILKPN" hidden="1">#REF!</definedName>
@@ -36,7 +37,7 @@
     <definedName name="wrn.Electricity._.Questionnaire." localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="wrn.Electricity._.Questionnaire." hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
   </definedNames>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -49,6 +50,24 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={D7F7A51F-98CC-4BD8-BF17-ABDD25DA4C1B}</author>
+  </authors>
+  <commentList>
+    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{D7F7A51F-98CC-4BD8-BF17-ABDD25DA4C1B}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    i.e. 51% reduction from the 2018 value (ca. 40 Mt based on https://www.epa.ie/pubs/reports/air/airemissions/ghg2018/Ireland%20GHG%201990-2018%20Final%20Inventory_April%202020.pdf )</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
@@ -74,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="89">
   <si>
     <t>LimType</t>
   </si>
@@ -291,9 +310,15 @@
     <t>UC - Each Region/All Periods</t>
   </si>
   <si>
+    <t>UC_RHSR</t>
+  </si>
+  <si>
     <t>UC - All Regions/Each Period</t>
   </si>
   <si>
+    <t>UC_RHS</t>
+  </si>
+  <si>
     <t>UC_desc</t>
   </si>
   <si>
@@ -312,49 +337,49 @@
     <t>Cset_Set</t>
   </si>
   <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>~UC_Sets: T_S:</t>
+  </si>
+  <si>
+    <t>Other_indexes</t>
+  </si>
+  <si>
     <t>ENV</t>
   </si>
   <si>
-    <t>Net zero CO2 emissions by 2050</t>
-  </si>
-  <si>
-    <t>UC_RHSRT</t>
-  </si>
-  <si>
-    <t>UC_RHSRT~0</t>
-  </si>
-  <si>
-    <t>UC_RHST~0</t>
-  </si>
-  <si>
-    <t>UC_RHST</t>
-  </si>
-  <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t>~UC_Sets: T_E:</t>
-  </si>
-  <si>
     <t>*CO2*,-*CO2S</t>
   </si>
   <si>
-    <t>Pset_CO</t>
-  </si>
-  <si>
-    <t>Pset_CI</t>
-  </si>
-  <si>
     <t>Pset_PN</t>
   </si>
   <si>
-    <t>*CO2*</t>
-  </si>
-  <si>
-    <t>-T-A*INT*</t>
+    <t>T-A*INT*,T-NAV*</t>
+  </si>
+  <si>
+    <t>~TFM_INS</t>
+  </si>
+  <si>
+    <t>TimeSlice</t>
+  </si>
+  <si>
+    <t>Attribute</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>COM_BNDNET</t>
+  </si>
+  <si>
+    <t>PWRCO2N</t>
   </si>
   <si>
     <t>UC_FLO</t>
+  </si>
+  <si>
+    <t>UC_COMNET</t>
   </si>
 </sst>
 </file>
@@ -366,7 +391,7 @@
     <numFmt numFmtId="164" formatCode="???,???.00"/>
     <numFmt numFmtId="165" formatCode="#,##0.0000"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -463,8 +488,21 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -501,6 +539,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="43"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="44"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -639,7 +689,7 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -661,7 +711,10 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="23">
     <cellStyle name="5x indented GHG Textfiels" xfId="3" xr:uid="{5F614CE9-C529-4323-B893-6D57470EC2CB}"/>
@@ -771,6 +824,12 @@
     <mc:Fallback/>
   </mc:AlternateContent>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Balyk, Olexandr" id="{1B80334F-2539-4DC6-A837-54D1ADCF10B1}" userId="Balyk, Olexandr" providerId="None"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1092,13 +1151,21 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="C7" dT="2021-03-03T22:33:41.43" personId="{1B80334F-2539-4DC6-A837-54D1ADCF10B1}" id="{D7F7A51F-98CC-4BD8-BF17-ABDD25DA4C1B}">
+    <text>i.e. 51% reduction from the 2018 value (ca. 40 Mt based on https://www.epa.ie/pubs/reports/air/airemissions/ghg2018/Ireland%20GHG%201990-2018%20Final%20Inventory_April%202020.pdf )</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42C030FF-C503-4743-9DBD-437AEB1E949D}">
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A3:AD37"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1860,19 +1927,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{011941A8-04BF-45E8-9F60-D4E07475AB4A}">
-  <dimension ref="A1:Q16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{011941A8-04BF-45E8-9F60-D4E07475AB4A}">
+  <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="8"/>
     <col min="2" max="2" width="14" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="12" width="9.140625" style="8"/>
+    <col min="3" max="3" width="25.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="12" width="9.140625" style="8"/>
     <col min="13" max="13" width="10.5703125" style="8" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12" style="8" bestFit="1" customWidth="1"/>
     <col min="15" max="16384" width="9.140625" style="8"/>
@@ -1941,10 +2009,9 @@
         <v>61</v>
       </c>
       <c r="C4" s="8" t="str">
-        <f xml:space="preserve"> _xlfn.TEXTJOIN("",TRUE,"UC_NetZeroCO2_by",C6)</f>
-        <v>UC_NetZeroCO2_by2050</v>
-      </c>
-      <c r="D4"/>
+        <f xml:space="preserve"> _xlfn.TEXTJOIN("_",TRUE,"UC","NetZero","CO2","2050")</f>
+        <v>UC_NetZero_CO2_2050</v>
+      </c>
       <c r="E4"/>
       <c r="F4"/>
       <c r="G4"/>
@@ -1962,12 +2029,12 @@
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5"/>
       <c r="B5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C5" t="s">
-        <v>73</v>
-      </c>
-      <c r="D5"/>
+        <v>68</v>
+      </c>
+      <c r="C5" t="str">
+        <f xml:space="preserve"> _xlfn.TEXTJOIN(" ",TRUE,"Net Zero CO2 by 2050")</f>
+        <v>Net Zero CO2 by 2050</v>
+      </c>
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5"/>
@@ -1984,92 +2051,104 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C6" s="8">
+        <v>2030</v>
+      </c>
+      <c r="D6" s="8">
         <v>2050</v>
+      </c>
+      <c r="E6" s="8">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C7" s="8">
+        <f>40000*0.49</f>
+        <v>19600</v>
+      </c>
+      <c r="D7" s="8">
         <v>0</v>
+      </c>
+      <c r="E7" s="8">
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>84</v>
+        <v>80</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>84</v>
+        <v>78</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>85</v>
+        <v>73</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
-        <v>71</v>
+        <v>0</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13"/>
       <c r="B13" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D13"/>
-      <c r="E13"/>
-      <c r="F13"/>
-      <c r="G13"/>
-      <c r="H13"/>
-      <c r="I13"/>
-      <c r="J13"/>
-      <c r="K13"/>
-      <c r="L13"/>
-      <c r="M13"/>
-      <c r="N13"/>
-      <c r="O13"/>
-      <c r="P13"/>
-      <c r="Q13"/>
+        <v>87</v>
+      </c>
+      <c r="C13" s="8">
+        <v>-1</v>
+      </c>
+      <c r="D13" s="8">
+        <v>-1</v>
+      </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14"/>
-      <c r="B14" s="8" t="s">
-        <v>86</v>
+      <c r="B14" t="s">
+        <v>88</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
-      <c r="D14"/>
+      <c r="D14" s="8">
+        <v>1</v>
+      </c>
       <c r="E14"/>
       <c r="F14"/>
       <c r="G14"/>
@@ -2122,99 +2201,117 @@
       <c r="P16"/>
       <c r="Q16"/>
     </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17"/>
+      <c r="B17"/>
+      <c r="C17"/>
+      <c r="D17"/>
+      <c r="E17"/>
+      <c r="F17"/>
+      <c r="G17"/>
+      <c r="H17"/>
+      <c r="I17"/>
+      <c r="J17"/>
+      <c r="K17"/>
+      <c r="L17"/>
+      <c r="M17"/>
+      <c r="N17"/>
+      <c r="O17"/>
+      <c r="P17"/>
+      <c r="Q17"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9318C9B-7F0A-410C-BCB5-F22D93E1F454}">
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="8"/>
-    <col min="2" max="2" width="29.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="13.5703125" style="8" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="8"/>
-    <col min="8" max="8" width="5.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="8"/>
-    <col min="10" max="10" width="12.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="8"/>
+    <col min="5" max="5" width="16.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="8"/>
+    <col min="9" max="9" width="13.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" style="8" customWidth="1"/>
     <col min="11" max="11" width="12" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="36.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="8"/>
+    <col min="12" max="12" width="27.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="str">
         <f>"~UC_Sets: R_E: "  &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3)</f>
         <v>~UC_Sets: R_E: IE</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I4" s="8" t="str">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H4" s="8" t="str">
         <f>IF(RIGHT(B2,1)&lt;&gt;" ","~UC_T","")</f>
         <v>~UC_T</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" s="12" t="s">
         <v>61</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="G5" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="J5" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="L5" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="9" t="s">
         <v>71</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="I5" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="J5" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="K5" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="L5" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="M5" s="12" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="9" t="s">
-        <v>69</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
@@ -2225,76 +2322,122 @@
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
       <c r="K6" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="L6" s="9"/>
-      <c r="M6" s="15"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="L6" s="15"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="str">
-        <f>VLOOKUP(B5, config!$B$4:$C$14,2,FALSE) &amp; "_Single"</f>
-        <v>UC_NetZeroCO2_by2050_Single</v>
+        <f>VLOOKUP(B$5, config!$B$4:$E$14,2,FALSE) &amp; "_Multi"</f>
+        <v>UC_NetZero_CO2_2050_Multi</v>
+      </c>
+      <c r="C7" s="8" t="str">
+        <f>VLOOKUP(C$5, config!$B$4:$E$14,2,FALSE)</f>
+        <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D7" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$C$14,2,FALSE)</f>
-        <v>*CO2*</v>
-      </c>
-      <c r="E7" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$C$14,2,FALSE)</f>
-        <v>-T-A*INT*</v>
-      </c>
-      <c r="F7" s="8" t="str">
-        <f>VLOOKUP(F$5, config!$B$4:$C$14,2,FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$E$14,2,FALSE)</f>
+        <v>ENV</v>
+      </c>
+      <c r="F7" s="8">
+        <f>VLOOKUP(F$5, config!$B$4:$E$14,2,FALSE)</f>
+        <v>2030</v>
+      </c>
+      <c r="H7" s="8" t="str">
+        <f>VLOOKUP(H$5, config!$B$4:$E$14,2,FALSE)</f>
+        <v>UP</v>
+      </c>
+      <c r="I7" s="8">
+        <f>VLOOKUP(I$5, config!$B$4:$E$14,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="K7" s="8">
+        <f>VLOOKUP("Value", config!$B$4:$E$14,2,FALSE)</f>
+        <v>19600</v>
+      </c>
+      <c r="L7" s="8" t="str">
+        <f>VLOOKUP(L$5, config!$B$4:$E$14,2,FALSE) &amp; " - Multi"</f>
+        <v>Net Zero CO2 by 2050 - Multi</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C8" s="8" t="str">
+        <f>VLOOKUP(C$5, config!$B$4:$E$14,2,FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
-      <c r="G7" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$C$14,2,FALSE)</f>
+      <c r="D8" s="8" t="str">
+        <f>VLOOKUP(D$5, config!$B$4:$E$14,2,FALSE)</f>
         <v>ENV</v>
       </c>
-      <c r="H7" s="8">
-        <f>VLOOKUP(H5, config!$B$4:$C$14,2,FALSE)</f>
+      <c r="E8" s="8" t="str">
+        <f>VLOOKUP(E$5, config!$B$4:$E$14,2,FALSE)</f>
+        <v>T-A*INT*,T-NAV*</v>
+      </c>
+      <c r="F8" s="8">
+        <f>VLOOKUP(F$5, config!$B$4:$E$14,2,FALSE)</f>
+        <v>2030</v>
+      </c>
+      <c r="J8" s="8">
+        <f>VLOOKUP(J$5, config!$B$4:$E$14,2,FALSE)</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C9" s="8" t="str">
+        <f>VLOOKUP(C$5, config!$B$4:$E$14,3,FALSE)</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="D9" s="8" t="str">
+        <f>VLOOKUP(D$5, config!$B$4:$E$14,3,FALSE)</f>
+        <v>ENV</v>
+      </c>
+      <c r="F9" s="8">
+        <f>VLOOKUP(F$5, config!$B$4:$E$14,3,FALSE)</f>
         <v>2050</v>
       </c>
-      <c r="I7" s="8" t="str">
-        <f>VLOOKUP(I5, config!$B$4:$C$14,2,FALSE)</f>
+      <c r="H9" s="8" t="str">
+        <f>VLOOKUP(H$5, config!$B$4:$E$14,3,FALSE)</f>
         <v>UP</v>
       </c>
-      <c r="J7" s="8">
-        <f>VLOOKUP(J5, config!$B$4:$C$14,2,FALSE)</f>
+      <c r="I9" s="8">
+        <f>VLOOKUP(I$5, config!$B$4:$E$14,3,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="K7" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$C$14,2,FALSE)*1000</f>
+      <c r="K9" s="8">
+        <f>VLOOKUP("Value", config!$B$4:$E$14,3,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="L7" s="8">
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C10" s="8" t="str">
+        <f>VLOOKUP(C$5, config!$B$4:$E$14,3,FALSE)</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="D10" s="8" t="str">
+        <f>VLOOKUP(D$5, config!$B$4:$E$14,3,FALSE)</f>
+        <v>ENV</v>
+      </c>
+      <c r="E10" s="8" t="str">
+        <f>VLOOKUP(E$5, config!$B$4:$E$14,3,FALSE)</f>
+        <v>T-A*INT*,T-NAV*</v>
+      </c>
+      <c r="F10" s="8">
+        <f>VLOOKUP(F$5, config!$B$4:$E$14,3,FALSE)</f>
+        <v>2050</v>
+      </c>
+      <c r="J10" s="8">
+        <f>VLOOKUP(J$5, config!$B$4:$E$14,3,FALSE)</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F11" s="8">
+        <f>VLOOKUP(F$5, config!$B$4:$E$14,4,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="K11" s="8">
+        <f>VLOOKUP("Value", config!$B$4:$E$14,4,FALSE)</f>
         <v>5</v>
-      </c>
-      <c r="M7" s="8" t="str">
-        <f>VLOOKUP(M5, config!$B$4:$C$14,2,FALSE) &amp; " - Single"</f>
-        <v>Net zero CO2 emissions by 2050 - Single</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C8" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$C$14,2,FALSE)</f>
-        <v>*CO2*</v>
-      </c>
-      <c r="F8" s="8" t="str">
-        <f>VLOOKUP(F$5, config!$B$4:$C$14,2,FALSE)</f>
-        <v>*CO2*,-*CO2S</v>
-      </c>
-      <c r="G8" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$C$14,2,FALSE)</f>
-        <v>ENV</v>
-      </c>
-      <c r="H8" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$C$14,2,FALSE)</f>
-        <v>2050</v>
-      </c>
-      <c r="J8" s="8">
-        <f>-VLOOKUP(J$5, config!$B$4:$C$14,2,FALSE)</f>
-        <v>-1</v>
       </c>
     </row>
   </sheetData>
@@ -2305,93 +2448,89 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6EC2971-91FC-4261-B0BB-58C7F43C1746}">
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="8"/>
-    <col min="2" max="2" width="28.5703125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="7.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="8"/>
-    <col min="10" max="10" width="12.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="36" style="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="8"/>
+    <col min="2" max="2" width="30.7109375" style="8" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="8"/>
+    <col min="5" max="5" width="16.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="8"/>
+    <col min="9" max="9" width="13.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" style="8" customWidth="1"/>
+    <col min="11" max="11" width="8.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="36.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="str">
         <f>"~UC_Sets: R_S: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!D3:AD3)</f>
         <v>~UC_Sets: R_S: National,IE-CW,IE-D,IE-KE,IE-KK,IE-LS,IE-LD,IE-LH,IE-MH,IE-OY,IE-WH,IE-WX,IE-WW,IE-CE,IE-CO,IE-KY,IE-LK,IE-TA,IE-WD,IE-G,IE-LM,IE-MO,IE-RN,IE-SO,IE-CN,IE-DL,IE-MN</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I4" s="8" t="str">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H4" s="8" t="str">
         <f>IF(RIGHT(B2,1)&lt;&gt;" ","~UC_T","")</f>
         <v>~UC_T</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" s="12" t="s">
         <v>61</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="G5" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="J5" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="L5" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="9" t="s">
         <v>71</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="I5" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="J5" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="K5" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="L5" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="M5" s="12" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="9" t="s">
-        <v>69</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
@@ -2402,80 +2541,205 @@
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
       <c r="K6" s="9" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="str">
-        <f>VLOOKUP(B5, config!$B$4:$C$14,2,FALSE) &amp; "_Multi"</f>
-        <v>UC_NetZeroCO2_by2050_Multi</v>
+        <f>VLOOKUP(B$5, config!$B$4:$E$14,2,FALSE) &amp; "_Multi"</f>
+        <v>UC_NetZero_CO2_2050_Multi</v>
+      </c>
+      <c r="C7" s="8" t="str">
+        <f>VLOOKUP(C$5, config!$B$4:$E$14,2,FALSE)</f>
+        <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D7" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$C$14,2,FALSE)</f>
-        <v>*CO2*</v>
-      </c>
-      <c r="E7" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$C$14,2,FALSE)</f>
-        <v>-T-A*INT*</v>
-      </c>
-      <c r="F7" s="8" t="str">
-        <f>VLOOKUP(F$5, config!$B$4:$C$14,2,FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$E$14,2,FALSE)</f>
+        <v>ENV</v>
+      </c>
+      <c r="F7" s="8">
+        <f>VLOOKUP(F$5, config!$B$4:$E$14,2,FALSE)</f>
+        <v>2030</v>
+      </c>
+      <c r="H7" s="8" t="str">
+        <f>VLOOKUP(H$5, config!$B$4:$E$14,2,FALSE)</f>
+        <v>UP</v>
+      </c>
+      <c r="I7" s="8">
+        <f>VLOOKUP(I$5, config!$B$4:$E$14,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="K7" s="8">
+        <f>VLOOKUP("Value", config!$B$4:$E$14,2,FALSE)</f>
+        <v>19600</v>
+      </c>
+      <c r="L7" s="8" t="str">
+        <f>VLOOKUP(L$5, config!$B$4:$E$14,2,FALSE) &amp; " - Multi"</f>
+        <v>Net Zero CO2 by 2050 - Multi</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C8" s="8" t="str">
+        <f>VLOOKUP(C$5, config!$B$4:$E$14,2,FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
-      <c r="G7" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$C$14,2,FALSE)</f>
+      <c r="D8" s="8" t="str">
+        <f>VLOOKUP(D$5, config!$B$4:$E$14,2,FALSE)</f>
         <v>ENV</v>
       </c>
-      <c r="H7" s="8">
-        <f>VLOOKUP(H5, config!$B$4:$C$14,2,FALSE)</f>
+      <c r="E8" s="8" t="str">
+        <f>VLOOKUP(E$5, config!$B$4:$E$14,2,FALSE)</f>
+        <v>T-A*INT*,T-NAV*</v>
+      </c>
+      <c r="F8" s="8">
+        <f>VLOOKUP(F$5, config!$B$4:$E$14,2,FALSE)</f>
+        <v>2030</v>
+      </c>
+      <c r="J8" s="8">
+        <f>VLOOKUP(J$5, config!$B$4:$E$14,2,FALSE)</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C9" s="8" t="str">
+        <f>VLOOKUP(C$5, config!$B$4:$E$14,3,FALSE)</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="D9" s="8" t="str">
+        <f>VLOOKUP(D$5, config!$B$4:$E$14,3,FALSE)</f>
+        <v>ENV</v>
+      </c>
+      <c r="F9" s="8">
+        <f>VLOOKUP(F$5, config!$B$4:$E$14,3,FALSE)</f>
         <v>2050</v>
       </c>
-      <c r="I7" s="8" t="str">
-        <f>VLOOKUP(I5, config!$B$4:$C$14,2,FALSE)</f>
+      <c r="H9" s="8" t="str">
+        <f>VLOOKUP(H$5, config!$B$4:$E$14,3,FALSE)</f>
         <v>UP</v>
       </c>
-      <c r="J7" s="8">
-        <f>VLOOKUP(J5, config!$B$4:$C$14,2,FALSE)</f>
+      <c r="I9" s="8">
+        <f>VLOOKUP(I$5, config!$B$4:$E$14,3,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="K7" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$C$14,2,FALSE)*1000</f>
+      <c r="K9" s="8">
+        <f>VLOOKUP("Value", config!$B$4:$E$14,3,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="L7" s="8">
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C10" s="8" t="str">
+        <f>VLOOKUP(C$5, config!$B$4:$E$14,3,FALSE)</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="D10" s="8" t="str">
+        <f>VLOOKUP(D$5, config!$B$4:$E$14,3,FALSE)</f>
+        <v>ENV</v>
+      </c>
+      <c r="E10" s="8" t="str">
+        <f>VLOOKUP(E$5, config!$B$4:$E$14,3,FALSE)</f>
+        <v>T-A*INT*,T-NAV*</v>
+      </c>
+      <c r="F10" s="8">
+        <f>VLOOKUP(F$5, config!$B$4:$E$14,3,FALSE)</f>
+        <v>2050</v>
+      </c>
+      <c r="J10" s="8">
+        <f>VLOOKUP(J$5, config!$B$4:$E$14,3,FALSE)</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F11" s="8">
+        <f>VLOOKUP(F$5, config!$B$4:$E$14,4,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="K11" s="8">
+        <f>VLOOKUP("Value", config!$B$4:$E$14,4,FALSE)</f>
         <v>5</v>
-      </c>
-      <c r="M7" s="8" t="str">
-        <f>VLOOKUP(M5, config!$B$4:$C$14,2,FALSE) &amp; " - Multi"</f>
-        <v>Net zero CO2 emissions by 2050 - Multi</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C8" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$C$14,2,FALSE)</f>
-        <v>*CO2*</v>
-      </c>
-      <c r="F8" s="8" t="str">
-        <f>VLOOKUP(F$5, config!$B$4:$C$14,2,FALSE)</f>
-        <v>*CO2*,-*CO2S</v>
-      </c>
-      <c r="G8" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$C$14,2,FALSE)</f>
-        <v>ENV</v>
-      </c>
-      <c r="H8" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$C$14,2,FALSE)</f>
-        <v>2050</v>
-      </c>
-      <c r="J8" s="8">
-        <f>-VLOOKUP(J$5, config!$B$4:$C$14,2,FALSE)</f>
-        <v>-1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2314F01-B0DB-448B-9217-DEB90E2D1CCA}">
+  <dimension ref="B2:H4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L29" sqref="L29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+    </row>
+    <row r="3" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="G3" s="18" t="str">
+        <f>Regions!C3</f>
+        <v>IE</v>
+      </c>
+      <c r="H3" s="18" t="str">
+        <f>Regions!D3</f>
+        <v>National</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="8"/>
+      <c r="C4" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="E4" s="8">
+        <v>0</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="G4" s="19">
+        <v>-1</v>
+      </c>
+      <c r="H4" s="19">
+        <f>G4</f>
+        <v>-1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fix errors in Net Zero scenarios
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SYS_ZeroCO2_2050.xlsx
+++ b/SuppXLS/Scen_SYS_ZeroCO2_2050.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F25FD08-7D51-4F02-A34E-10DBB506647D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A85636D9-A0BA-4A84-AAA5-18824A647F3D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="15" r:id="rId1"/>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="89">
   <si>
     <t>LimType</t>
   </si>
@@ -310,15 +310,9 @@
     <t>UC - Each Region/All Periods</t>
   </si>
   <si>
-    <t>UC_RHSR</t>
-  </si>
-  <si>
     <t>UC - All Regions/Each Period</t>
   </si>
   <si>
-    <t>UC_RHS</t>
-  </si>
-  <si>
     <t>UC_desc</t>
   </si>
   <si>
@@ -380,6 +374,12 @@
   </si>
   <si>
     <t>UC_COMNET</t>
+  </si>
+  <si>
+    <t>UC_RHSRTS</t>
+  </si>
+  <si>
+    <t>UC_RHSTS</t>
   </si>
 </sst>
 </file>
@@ -391,7 +391,7 @@
     <numFmt numFmtId="164" formatCode="???,???.00"/>
     <numFmt numFmtId="165" formatCode="#,##0.0000"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -494,12 +494,6 @@
       <color indexed="12"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="10">
@@ -1164,7 +1158,7 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A3:AD37"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -1931,7 +1925,7 @@
   <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2029,7 +2023,7 @@
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5"/>
       <c r="B5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C5" t="str">
         <f xml:space="preserve"> _xlfn.TEXTJOIN(" ",TRUE,"Net Zero CO2 by 2050")</f>
@@ -2051,7 +2045,7 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C6" s="8">
         <v>2030</v>
@@ -2065,7 +2059,7 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C7" s="8">
         <f>40000*0.49</f>
@@ -2080,13 +2074,13 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -2094,26 +2088,26 @@
         <v>62</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -2121,15 +2115,15 @@
         <v>0</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C13" s="8">
         <v>-1</v>
@@ -2141,7 +2135,7 @@
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14"/>
       <c r="B14" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -2229,52 +2223,51 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9318C9B-7F0A-410C-BCB5-F22D93E1F454}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="8"/>
-    <col min="2" max="2" width="31" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="8"/>
+    <col min="4" max="4" width="8.85546875" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="8"/>
-    <col min="9" max="9" width="13.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" style="8" customWidth="1"/>
-    <col min="11" max="11" width="12" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="27.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="8"/>
+    <col min="6" max="6" width="5.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="8"/>
+    <col min="8" max="8" width="12.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="str">
         <f>"~UC_Sets: R_E: "  &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3)</f>
         <v>~UC_Sets: R_E: IE</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H4" s="8" t="str">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G4" s="8" t="str">
         <f>IF(RIGHT(B2,1)&lt;&gt;" ","~UC_T","")</f>
         <v>~UC_T</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" s="12" t="s">
         <v>61</v>
       </c>
@@ -2282,36 +2275,33 @@
         <v>62</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="H5" s="13" t="s">
         <v>0</v>
       </c>
+      <c r="H5" s="14" t="s">
+        <v>86</v>
+      </c>
       <c r="I5" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="J5" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="J5" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="K5" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="L5" s="12" t="s">
+      <c r="K5" s="12" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
@@ -2320,16 +2310,15 @@
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="L6" s="15"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J6" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="K6" s="15"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="str">
-        <f>VLOOKUP(B$5, config!$B$4:$E$14,2,FALSE) &amp; "_Multi"</f>
-        <v>UC_NetZero_CO2_2050_Multi</v>
+        <f>VLOOKUP(B$5, config!$B$4:$E$14,2,FALSE) &amp; "_Single"</f>
+        <v>UC_NetZero_CO2_2050_Single</v>
       </c>
       <c r="C7" s="8" t="str">
         <f>VLOOKUP(C$5, config!$B$4:$E$14,2,FALSE)</f>
@@ -2343,24 +2332,24 @@
         <f>VLOOKUP(F$5, config!$B$4:$E$14,2,FALSE)</f>
         <v>2030</v>
       </c>
-      <c r="H7" s="8" t="str">
+      <c r="G7" s="8" t="str">
+        <f>VLOOKUP(G$5, config!$B$4:$E$14,2,FALSE)</f>
+        <v>UP</v>
+      </c>
+      <c r="H7" s="8">
         <f>VLOOKUP(H$5, config!$B$4:$E$14,2,FALSE)</f>
-        <v>UP</v>
-      </c>
-      <c r="I7" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$E$14,2,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="K7" s="8">
+      <c r="J7" s="8">
         <f>VLOOKUP("Value", config!$B$4:$E$14,2,FALSE)</f>
         <v>19600</v>
       </c>
-      <c r="L7" s="8" t="str">
-        <f>VLOOKUP(L$5, config!$B$4:$E$14,2,FALSE) &amp; " - Multi"</f>
-        <v>Net Zero CO2 by 2050 - Multi</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K7" s="8" t="str">
+        <f>VLOOKUP(K$5, config!$B$4:$E$14,2,FALSE) &amp; " - Single"</f>
+        <v>Net Zero CO2 by 2050 - Single</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C8" s="8" t="str">
         <f>VLOOKUP(C$5, config!$B$4:$E$14,2,FALSE)</f>
         <v>*CO2*,-*CO2S</v>
@@ -2377,12 +2366,12 @@
         <f>VLOOKUP(F$5, config!$B$4:$E$14,2,FALSE)</f>
         <v>2030</v>
       </c>
-      <c r="J8" s="8">
-        <f>VLOOKUP(J$5, config!$B$4:$E$14,2,FALSE)</f>
+      <c r="I8" s="8">
+        <f>VLOOKUP(I$5, config!$B$4:$E$14,2,FALSE)</f>
         <v>-1</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C9" s="8" t="str">
         <f>VLOOKUP(C$5, config!$B$4:$E$14,3,FALSE)</f>
         <v>*CO2*,-*CO2S</v>
@@ -2395,20 +2384,20 @@
         <f>VLOOKUP(F$5, config!$B$4:$E$14,3,FALSE)</f>
         <v>2050</v>
       </c>
-      <c r="H9" s="8" t="str">
+      <c r="G9" s="8" t="str">
+        <f>VLOOKUP(G$5, config!$B$4:$E$14,3,FALSE)</f>
+        <v>UP</v>
+      </c>
+      <c r="H9" s="8">
         <f>VLOOKUP(H$5, config!$B$4:$E$14,3,FALSE)</f>
-        <v>UP</v>
-      </c>
-      <c r="I9" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$E$14,3,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="K9" s="8">
+      <c r="J9" s="8">
         <f>VLOOKUP("Value", config!$B$4:$E$14,3,FALSE)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C10" s="8" t="str">
         <f>VLOOKUP(C$5, config!$B$4:$E$14,3,FALSE)</f>
         <v>*CO2*,-*CO2S</v>
@@ -2425,17 +2414,17 @@
         <f>VLOOKUP(F$5, config!$B$4:$E$14,3,FALSE)</f>
         <v>2050</v>
       </c>
-      <c r="J10" s="8">
-        <f>VLOOKUP(J$5, config!$B$4:$E$14,3,FALSE)</f>
+      <c r="I10" s="8">
+        <f>VLOOKUP(I$5, config!$B$4:$E$14,3,FALSE)</f>
         <v>-1</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F11" s="8">
         <f>VLOOKUP(F$5, config!$B$4:$E$14,4,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="K11" s="8">
+      <c r="J11" s="8">
         <f>VLOOKUP("Value", config!$B$4:$E$14,4,FALSE)</f>
         <v>5</v>
       </c>
@@ -2448,52 +2437,51 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6EC2971-91FC-4261-B0BB-58C7F43C1746}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="8"/>
-    <col min="2" max="2" width="30.7109375" style="8" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" style="8" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="8"/>
+    <col min="4" max="4" width="8.85546875" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="8"/>
-    <col min="9" max="9" width="13.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" style="8" customWidth="1"/>
-    <col min="11" max="11" width="8.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="36.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="8"/>
+    <col min="6" max="6" width="5.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="str">
         <f>"~UC_Sets: R_S: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!D3:AD3)</f>
         <v>~UC_Sets: R_S: National,IE-CW,IE-D,IE-KE,IE-KK,IE-LS,IE-LD,IE-LH,IE-MH,IE-OY,IE-WH,IE-WX,IE-WW,IE-CE,IE-CO,IE-KY,IE-LK,IE-TA,IE-WD,IE-G,IE-LM,IE-MO,IE-RN,IE-SO,IE-CN,IE-DL,IE-MN</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H4" s="8" t="str">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G4" s="8" t="str">
         <f>IF(RIGHT(B2,1)&lt;&gt;" ","~UC_T","")</f>
         <v>~UC_T</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" s="12" t="s">
         <v>61</v>
       </c>
@@ -2501,36 +2489,33 @@
         <v>62</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="H5" s="13" t="s">
         <v>0</v>
       </c>
+      <c r="H5" s="14" t="s">
+        <v>86</v>
+      </c>
       <c r="I5" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="J5" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="J5" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="K5" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="L5" s="12" t="s">
+      <c r="K5" s="12" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
@@ -2539,13 +2524,12 @@
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="L6" s="9"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J6" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="K6" s="9"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="str">
         <f>VLOOKUP(B$5, config!$B$4:$E$14,2,FALSE) &amp; "_Multi"</f>
         <v>UC_NetZero_CO2_2050_Multi</v>
@@ -2562,24 +2546,24 @@
         <f>VLOOKUP(F$5, config!$B$4:$E$14,2,FALSE)</f>
         <v>2030</v>
       </c>
-      <c r="H7" s="8" t="str">
+      <c r="G7" s="8" t="str">
+        <f>VLOOKUP(G$5, config!$B$4:$E$14,2,FALSE)</f>
+        <v>UP</v>
+      </c>
+      <c r="H7" s="8">
         <f>VLOOKUP(H$5, config!$B$4:$E$14,2,FALSE)</f>
-        <v>UP</v>
-      </c>
-      <c r="I7" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$E$14,2,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="K7" s="8">
+      <c r="J7" s="8">
         <f>VLOOKUP("Value", config!$B$4:$E$14,2,FALSE)</f>
         <v>19600</v>
       </c>
-      <c r="L7" s="8" t="str">
-        <f>VLOOKUP(L$5, config!$B$4:$E$14,2,FALSE) &amp; " - Multi"</f>
+      <c r="K7" s="8" t="str">
+        <f>VLOOKUP(K$5, config!$B$4:$E$14,2,FALSE) &amp; " - Multi"</f>
         <v>Net Zero CO2 by 2050 - Multi</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C8" s="8" t="str">
         <f>VLOOKUP(C$5, config!$B$4:$E$14,2,FALSE)</f>
         <v>*CO2*,-*CO2S</v>
@@ -2596,12 +2580,12 @@
         <f>VLOOKUP(F$5, config!$B$4:$E$14,2,FALSE)</f>
         <v>2030</v>
       </c>
-      <c r="J8" s="8">
-        <f>VLOOKUP(J$5, config!$B$4:$E$14,2,FALSE)</f>
+      <c r="I8" s="8">
+        <f>VLOOKUP(I$5, config!$B$4:$E$14,2,FALSE)</f>
         <v>-1</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C9" s="8" t="str">
         <f>VLOOKUP(C$5, config!$B$4:$E$14,3,FALSE)</f>
         <v>*CO2*,-*CO2S</v>
@@ -2614,20 +2598,20 @@
         <f>VLOOKUP(F$5, config!$B$4:$E$14,3,FALSE)</f>
         <v>2050</v>
       </c>
-      <c r="H9" s="8" t="str">
+      <c r="G9" s="8" t="str">
+        <f>VLOOKUP(G$5, config!$B$4:$E$14,3,FALSE)</f>
+        <v>UP</v>
+      </c>
+      <c r="H9" s="8">
         <f>VLOOKUP(H$5, config!$B$4:$E$14,3,FALSE)</f>
-        <v>UP</v>
-      </c>
-      <c r="I9" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$E$14,3,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="K9" s="8">
+      <c r="J9" s="8">
         <f>VLOOKUP("Value", config!$B$4:$E$14,3,FALSE)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C10" s="8" t="str">
         <f>VLOOKUP(C$5, config!$B$4:$E$14,3,FALSE)</f>
         <v>*CO2*,-*CO2S</v>
@@ -2644,17 +2628,17 @@
         <f>VLOOKUP(F$5, config!$B$4:$E$14,3,FALSE)</f>
         <v>2050</v>
       </c>
-      <c r="J10" s="8">
-        <f>VLOOKUP(J$5, config!$B$4:$E$14,3,FALSE)</f>
+      <c r="I10" s="8">
+        <f>VLOOKUP(I$5, config!$B$4:$E$14,3,FALSE)</f>
         <v>-1</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F11" s="8">
         <f>VLOOKUP(F$5, config!$B$4:$E$14,4,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="K11" s="8">
+      <c r="J11" s="8">
         <f>VLOOKUP("Value", config!$B$4:$E$14,4,FALSE)</f>
         <v>5</v>
       </c>
@@ -2683,7 +2667,7 @@
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" s="16" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
@@ -2694,16 +2678,16 @@
     </row>
     <row r="3" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="17" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C3" s="17" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F3" s="17" t="s">
         <v>62</v>
@@ -2720,16 +2704,16 @@
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="8"/>
       <c r="C4" s="10" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E4" s="8">
         <v>0</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G4" s="19">
         <v>-1</v>

</xml_diff>